<commit_message>
Cleaned up some methods, removed the default save behaviour, finished the implementation of the DELETE ROW button
</commit_message>
<xml_diff>
--- a/test/Excel C# Test.xlsx
+++ b/test/Excel C# Test.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dev\Unknown\FirstExcelAddIn\FirstExcelAddIn\test\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" activeTab="1"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="3" r:id="rId1"/>
     <sheet name="Input" sheetId="2" r:id="rId2"/>
     <sheet name="Market Assumptions" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1"/>
+  <calcPr calcId="152511" iterate="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -218,7 +223,7 @@
     <t>Tenant 3</t>
   </si>
   <si>
-    <t>Tenant 4</t>
+    <t>Tenant 2</t>
   </si>
 </sst>
 </file>
@@ -717,7 +722,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -816,8 +821,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -916,7 +921,7 @@
     </row>
     <row r="4" spans="1:10" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="7"/>
@@ -930,7 +935,7 @@
     </row>
     <row r="5" spans="1:10" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="7"/>
@@ -960,8 +965,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:DL13"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2908,7 +2913,7 @@
     <row r="10" spans="1:116" s="2" customFormat="1" ht="12.95" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="str">
         <f>Input!A4</f>
-        <v>Tenant 3</v>
+        <v>Tenant 2</v>
       </c>
       <c r="D10" s="13">
         <f>Input!C4</f>
@@ -3354,7 +3359,7 @@
     <row r="11" spans="1:116" s="2" customFormat="1" ht="12.95" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="str">
         <f>Input!A5</f>
-        <v>Tenant 4</v>
+        <v>Tenant 3</v>
       </c>
       <c r="D11" s="13">
         <f>Input!C5</f>
@@ -4202,7 +4207,7 @@
         <v>0</v>
       </c>
       <c r="DI13" s="13">
-        <f t="shared" ref="DI13:EN13" si="9">SUMPRODUCT(DI9:DI12,$D$9:$D$12)</f>
+        <f t="shared" ref="DI13:DL13" si="9">SUMPRODUCT(DI9:DI12,$D$9:$D$12)</f>
         <v>0</v>
       </c>
       <c r="DJ13" s="13">

</xml_diff>